<commit_message>
working on pso documentation
</commit_message>
<xml_diff>
--- a/hw6_PSO/Results2.xlsx
+++ b/hw6_PSO/Results2.xlsx
@@ -417,25 +417,25 @@
         <v>10</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>0.718</v>
+        <v>809.687</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>390275.222</v>
+        <v>11237183.211</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>3902475.076</v>
+        <v>23340243.403</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>1170733.285</v>
+        <v>6379505.299</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>3.576</v>
+        <v>4.449</v>
       </c>
       <c r="G4" t="n">
-        <v>3.655</v>
+        <v>4.697</v>
       </c>
       <c r="H4" t="n">
-        <v>3.857</v>
+        <v>5.365</v>
       </c>
     </row>
     <row r="5">
@@ -443,25 +443,25 @@
         <v>30</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>29</v>
+        <v>154862177.941</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>29</v>
+        <v>213142558.437</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>29</v>
+        <v>269288404.216</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>0</v>
+        <v>39778983.974</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>20.957</v>
+        <v>37.047</v>
       </c>
       <c r="G5" t="n">
-        <v>21.54</v>
+        <v>37.459</v>
       </c>
       <c r="H5" t="n">
-        <v>22.038</v>
+        <v>37.788</v>
       </c>
     </row>
     <row r="6">
@@ -469,25 +469,25 @@
         <v>50</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>372345192.619</v>
+        <v>372451257.346</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>427387668.999</v>
+        <v>423759402.813</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>564571752.4</v>
+        <v>514936531.617</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>52384447.808</v>
+        <v>41476770.343</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>81.514</v>
+        <v>101.056</v>
       </c>
       <c r="G6" t="n">
-        <v>85.15000000000001</v>
+        <v>102.133</v>
       </c>
       <c r="H6" t="n">
-        <v>88.959</v>
+        <v>106.064</v>
       </c>
     </row>
     <row r="7">
@@ -552,25 +552,25 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>0</v>
+        <v>0.007</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>0</v>
+        <v>7592.682</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>0</v>
+        <v>13009.57</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>0</v>
+        <v>4979.597</v>
       </c>
       <c r="F10" s="1" t="n">
-        <v>1.532</v>
+        <v>2.045</v>
       </c>
       <c r="G10" t="n">
-        <v>1.764</v>
+        <v>2.126</v>
       </c>
       <c r="H10" t="n">
-        <v>2.091</v>
+        <v>2.287</v>
       </c>
     </row>
     <row r="11">
@@ -578,25 +578,25 @@
         <v>30</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>0</v>
+        <v>17658.604</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>18830.998</v>
+        <v>56757.67</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>73022.25199999999</v>
+        <v>66604.288</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>29188.32</v>
+        <v>13810.082</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>10.902</v>
+        <v>13.757</v>
       </c>
       <c r="G11" t="n">
-        <v>11.979</v>
+        <v>14.278</v>
       </c>
       <c r="H11" t="n">
-        <v>13.843</v>
+        <v>14.764</v>
       </c>
     </row>
     <row r="12">
@@ -604,25 +604,25 @@
         <v>50</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>3.867</v>
+        <v>102100.83</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>106877.157</v>
+        <v>116331.477</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>129563.617</v>
+        <v>126348.038</v>
       </c>
       <c r="E12" s="1" t="n">
-        <v>36214.941</v>
+        <v>7407.646</v>
       </c>
       <c r="F12" s="1" t="n">
-        <v>29.053</v>
+        <v>34.922</v>
       </c>
       <c r="G12" t="n">
-        <v>31.056</v>
+        <v>35.352</v>
       </c>
       <c r="H12" t="n">
-        <v>32.958</v>
+        <v>36.189</v>
       </c>
     </row>
     <row r="13">
@@ -687,25 +687,25 @@
         <v>10</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>0</v>
+        <v>2.776</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>0.116</v>
+        <v>15.715</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>1.155</v>
+        <v>19.775</v>
       </c>
       <c r="E16" s="1" t="n">
-        <v>0.347</v>
+        <v>6.371</v>
       </c>
       <c r="F16" s="1" t="n">
-        <v>3.071</v>
+        <v>3.99</v>
       </c>
       <c r="G16" t="n">
-        <v>3.155</v>
+        <v>4.054</v>
       </c>
       <c r="H16" t="n">
-        <v>3.31</v>
+        <v>4.176</v>
       </c>
     </row>
     <row r="17">
@@ -713,25 +713,25 @@
         <v>30</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>1.34</v>
+        <v>20.134</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>9.526999999999999</v>
+        <v>20.536</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>20.417</v>
+        <v>20.774</v>
       </c>
       <c r="E17" s="1" t="n">
-        <v>7.166</v>
+        <v>0.158</v>
       </c>
       <c r="F17" s="1" t="n">
-        <v>22.673</v>
+        <v>28.267</v>
       </c>
       <c r="G17" t="n">
-        <v>25.178</v>
+        <v>28.653</v>
       </c>
       <c r="H17" t="n">
-        <v>29.165</v>
+        <v>29.258</v>
       </c>
     </row>
     <row r="18">
@@ -739,25 +739,25 @@
         <v>50</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>18.311</v>
+        <v>20.549</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>20.243</v>
+        <v>20.724</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>20.811</v>
+        <v>20.869</v>
       </c>
       <c r="E18" s="1" t="n">
-        <v>0.956</v>
+        <v>0.095</v>
       </c>
       <c r="F18" s="1" t="n">
-        <v>60.583</v>
+        <v>73.71299999999999</v>
       </c>
       <c r="G18" t="n">
-        <v>64.54600000000001</v>
+        <v>75.56100000000001</v>
       </c>
       <c r="H18" t="n">
-        <v>68.012</v>
+        <v>78.52500000000001</v>
       </c>
     </row>
     <row r="19">
@@ -822,25 +822,25 @@
         <v>10</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>0.081</v>
+        <v>1.065</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>0.169</v>
+        <v>74.062</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>0.28</v>
+        <v>116.332</v>
       </c>
       <c r="E22" s="1" t="n">
-        <v>0.061</v>
+        <v>39.959</v>
       </c>
       <c r="F22" s="1" t="n">
-        <v>3.3</v>
+        <v>4.074</v>
       </c>
       <c r="G22" t="n">
-        <v>4.042</v>
+        <v>4.239</v>
       </c>
       <c r="H22" t="n">
-        <v>4.51</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="23">
@@ -848,25 +848,25 @@
         <v>30</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>0.007</v>
+        <v>446.43</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>228.708</v>
+        <v>543.7809999999999</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>630.432</v>
+        <v>617.864</v>
       </c>
       <c r="E23" s="1" t="n">
-        <v>282.108</v>
+        <v>50.938</v>
       </c>
       <c r="F23" s="1" t="n">
-        <v>25.401</v>
+        <v>30.074</v>
       </c>
       <c r="G23" t="n">
-        <v>26.921</v>
+        <v>31.088</v>
       </c>
       <c r="H23" t="n">
-        <v>30.285</v>
+        <v>32.174</v>
       </c>
     </row>
     <row r="24">
@@ -874,25 +874,25 @@
         <v>50</v>
       </c>
       <c r="B24" s="1" t="n">
-        <v>948.244</v>
+        <v>989.727</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>1053.5</v>
+        <v>1056.827</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>1180.919</v>
+        <v>1130.995</v>
       </c>
       <c r="E24" s="1" t="n">
-        <v>64.91</v>
+        <v>43.659</v>
       </c>
       <c r="F24" s="1" t="n">
-        <v>64.006</v>
+        <v>80.224</v>
       </c>
       <c r="G24" t="n">
-        <v>66.931</v>
+        <v>82.98699999999999</v>
       </c>
       <c r="H24" t="n">
-        <v>74.236</v>
+        <v>85.14100000000001</v>
       </c>
     </row>
     <row r="25">
@@ -957,25 +957,25 @@
         <v>10</v>
       </c>
       <c r="B28" s="1" t="n">
-        <v>2.985</v>
+        <v>93.831</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>13.432</v>
+        <v>206250.984</v>
       </c>
       <c r="D28" s="1" t="n">
-        <v>35.818</v>
+        <v>364318.054</v>
       </c>
       <c r="E28" s="1" t="n">
-        <v>8.304</v>
+        <v>119098.041</v>
       </c>
       <c r="F28" s="1" t="n">
-        <v>2.977</v>
+        <v>3.78</v>
       </c>
       <c r="G28" t="n">
-        <v>3.093</v>
+        <v>3.872</v>
       </c>
       <c r="H28" t="n">
-        <v>3.652</v>
+        <v>3.971</v>
       </c>
     </row>
     <row r="29">
@@ -983,25 +983,25 @@
         <v>30</v>
       </c>
       <c r="B29" s="1" t="n">
-        <v>41.87</v>
+        <v>1262383.423</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>366393.929</v>
+        <v>1518041.319</v>
       </c>
       <c r="D29" s="1" t="n">
-        <v>1840626.356</v>
+        <v>1809166.501</v>
       </c>
       <c r="E29" s="1" t="n">
-        <v>732424.041</v>
+        <v>179280.57</v>
       </c>
       <c r="F29" s="1" t="n">
-        <v>22.784</v>
+        <v>28.632</v>
       </c>
       <c r="G29" t="n">
-        <v>23.651</v>
+        <v>29.165</v>
       </c>
       <c r="H29" t="n">
-        <v>24.491</v>
+        <v>30.322</v>
       </c>
     </row>
     <row r="30">
@@ -1009,25 +1009,25 @@
         <v>50</v>
       </c>
       <c r="B30" s="1" t="n">
-        <v>468.99</v>
+        <v>2741063.758</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>2453097.392</v>
+        <v>3172679.587</v>
       </c>
       <c r="D30" s="1" t="n">
-        <v>3394777.118</v>
+        <v>3389324.577</v>
       </c>
       <c r="E30" s="1" t="n">
-        <v>1242255.09</v>
+        <v>196937.608</v>
       </c>
       <c r="F30" s="1" t="n">
-        <v>62.361</v>
+        <v>76.726</v>
       </c>
       <c r="G30" t="n">
-        <v>65.773</v>
+        <v>78.09399999999999</v>
       </c>
       <c r="H30" t="n">
-        <v>70.785</v>
+        <v>80.235</v>
       </c>
     </row>
     <row r="31">
@@ -1092,25 +1092,25 @@
         <v>10</v>
       </c>
       <c r="B34" s="1" t="n">
-        <v>-3.065</v>
+        <v>12.3</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>2273442.928</v>
+        <v>3863847.826</v>
       </c>
       <c r="D34" s="1" t="n">
-        <v>15389408.388</v>
+        <v>18455086.861</v>
       </c>
       <c r="E34" s="1" t="n">
-        <v>4889765.852</v>
+        <v>5494331.53</v>
       </c>
       <c r="F34" s="1" t="n">
-        <v>5.798</v>
+        <v>7.965</v>
       </c>
       <c r="G34" t="n">
-        <v>6.182</v>
+        <v>8.321999999999999</v>
       </c>
       <c r="H34" t="n">
-        <v>7.254</v>
+        <v>8.760999999999999</v>
       </c>
     </row>
     <row r="35">
@@ -1118,25 +1118,25 @@
         <v>30</v>
       </c>
       <c r="B35" s="1" t="n">
-        <v>-1.022</v>
+        <v>208679432.699</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>251187238.995</v>
+        <v>441762958.29</v>
       </c>
       <c r="D35" s="1" t="n">
-        <v>670446493.8430001</v>
+        <v>615676602.46</v>
       </c>
       <c r="E35" s="1" t="n">
-        <v>261969196.901</v>
+        <v>105949769.312</v>
       </c>
       <c r="F35" s="1" t="n">
-        <v>49.613</v>
+        <v>65.405</v>
       </c>
       <c r="G35" t="n">
-        <v>56.328</v>
+        <v>67.39100000000001</v>
       </c>
       <c r="H35" t="n">
-        <v>61.644</v>
+        <v>70.60599999999999</v>
       </c>
     </row>
     <row r="36">
@@ -1144,25 +1144,25 @@
         <v>50</v>
       </c>
       <c r="B36" s="1" t="n">
-        <v>915027566.159</v>
+        <v>817405757.696</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>1044265014.822</v>
+        <v>1031807824.065</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>1247332716.111</v>
+        <v>1221361116.583</v>
       </c>
       <c r="E36" s="1" t="n">
-        <v>102118207.001</v>
+        <v>121164612.685</v>
       </c>
       <c r="F36" s="1" t="n">
-        <v>144.241</v>
+        <v>179.077</v>
       </c>
       <c r="G36" t="n">
-        <v>154.673</v>
+        <v>183.083</v>
       </c>
       <c r="H36" t="n">
-        <v>173.673</v>
+        <v>189.299</v>
       </c>
     </row>
     <row r="37">

</xml_diff>

<commit_message>
box plots for 3 first algorithms added
</commit_message>
<xml_diff>
--- a/hw6_PSO/Results2.xlsx
+++ b/hw6_PSO/Results2.xlsx
@@ -417,25 +417,25 @@
         <v>10</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>809.687</v>
+        <v>0.371</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>11237183.211</v>
+        <v>2.897</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>23340243.403</v>
+        <v>7.328</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>6379505.299</v>
+        <v>2.22</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>4.449</v>
+        <v>3.802</v>
       </c>
       <c r="G4" t="n">
-        <v>4.697</v>
+        <v>4.189</v>
       </c>
       <c r="H4" t="n">
-        <v>5.365</v>
+        <v>4.546</v>
       </c>
     </row>
     <row r="5">
@@ -443,25 +443,25 @@
         <v>30</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>154862177.941</v>
+        <v>46.455</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>213142558.437</v>
+        <v>109172085.958</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>269288404.216</v>
+        <v>274556070.182</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>39778983.974</v>
+        <v>115084333.978</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>37.047</v>
+        <v>32.878</v>
       </c>
       <c r="G5" t="n">
-        <v>37.459</v>
+        <v>35.162</v>
       </c>
       <c r="H5" t="n">
-        <v>37.788</v>
+        <v>36.928</v>
       </c>
     </row>
     <row r="6">
@@ -469,25 +469,25 @@
         <v>50</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>372451257.346</v>
+        <v>423.671</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>423759402.813</v>
+        <v>300610421.643</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>514936531.617</v>
+        <v>488700241.637</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>41476770.343</v>
+        <v>201811437.079</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>101.056</v>
+        <v>90.601</v>
       </c>
       <c r="G6" t="n">
-        <v>102.133</v>
+        <v>92.941</v>
       </c>
       <c r="H6" t="n">
-        <v>106.064</v>
+        <v>97.233</v>
       </c>
     </row>
     <row r="7">
@@ -552,25 +552,25 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>0.007</v>
+        <v>0</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>7592.682</v>
+        <v>1020.734</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>13009.57</v>
+        <v>6461.495</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>4979.597</v>
+        <v>2129.866</v>
       </c>
       <c r="F10" s="1" t="n">
-        <v>2.045</v>
+        <v>1.594</v>
       </c>
       <c r="G10" t="n">
-        <v>2.126</v>
+        <v>1.804</v>
       </c>
       <c r="H10" t="n">
-        <v>2.287</v>
+        <v>2.09</v>
       </c>
     </row>
     <row r="11">
@@ -578,25 +578,25 @@
         <v>30</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>17658.604</v>
+        <v>0</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>56757.67</v>
+        <v>30204.419</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>66604.288</v>
+        <v>69741.77800000001</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>13810.082</v>
+        <v>30895.739</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>13.757</v>
+        <v>12.651</v>
       </c>
       <c r="G11" t="n">
-        <v>14.278</v>
+        <v>13.408</v>
       </c>
       <c r="H11" t="n">
-        <v>14.764</v>
+        <v>15.106</v>
       </c>
     </row>
     <row r="12">
@@ -604,25 +604,25 @@
         <v>50</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>102100.83</v>
+        <v>108094.892</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>116331.477</v>
+        <v>116438.343</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>126348.038</v>
+        <v>123925.061</v>
       </c>
       <c r="E12" s="1" t="n">
-        <v>7407.646</v>
+        <v>5939.353</v>
       </c>
       <c r="F12" s="1" t="n">
-        <v>34.922</v>
+        <v>30.852</v>
       </c>
       <c r="G12" t="n">
-        <v>35.352</v>
+        <v>34.752</v>
       </c>
       <c r="H12" t="n">
-        <v>36.189</v>
+        <v>37.93</v>
       </c>
     </row>
     <row r="13">
@@ -687,25 +687,25 @@
         <v>10</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>2.776</v>
+        <v>0</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>15.715</v>
+        <v>3.738</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>19.775</v>
+        <v>19.317</v>
       </c>
       <c r="E16" s="1" t="n">
-        <v>6.371</v>
+        <v>7.481</v>
       </c>
       <c r="F16" s="1" t="n">
-        <v>3.99</v>
+        <v>3.478</v>
       </c>
       <c r="G16" t="n">
-        <v>4.054</v>
+        <v>3.738</v>
       </c>
       <c r="H16" t="n">
-        <v>4.176</v>
+        <v>4.257</v>
       </c>
     </row>
     <row r="17">
@@ -713,25 +713,25 @@
         <v>30</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>20.134</v>
+        <v>16.644</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>20.536</v>
+        <v>19.144</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>20.774</v>
+        <v>20.699</v>
       </c>
       <c r="E17" s="1" t="n">
-        <v>0.158</v>
+        <v>1.339</v>
       </c>
       <c r="F17" s="1" t="n">
-        <v>28.267</v>
+        <v>23.336</v>
       </c>
       <c r="G17" t="n">
-        <v>28.653</v>
+        <v>24.62</v>
       </c>
       <c r="H17" t="n">
-        <v>29.258</v>
+        <v>25.715</v>
       </c>
     </row>
     <row r="18">
@@ -739,25 +739,25 @@
         <v>50</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>20.549</v>
+        <v>19.094</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>20.724</v>
+        <v>20.136</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>20.869</v>
+        <v>20.863</v>
       </c>
       <c r="E18" s="1" t="n">
-        <v>0.095</v>
+        <v>0.75</v>
       </c>
       <c r="F18" s="1" t="n">
-        <v>73.71299999999999</v>
+        <v>60.857</v>
       </c>
       <c r="G18" t="n">
-        <v>75.56100000000001</v>
+        <v>64.611</v>
       </c>
       <c r="H18" t="n">
-        <v>78.52500000000001</v>
+        <v>75.34099999999999</v>
       </c>
     </row>
     <row r="19">
@@ -822,25 +822,25 @@
         <v>10</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>1.065</v>
+        <v>0.034</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>74.062</v>
+        <v>37.907</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>116.332</v>
+        <v>138.325</v>
       </c>
       <c r="E22" s="1" t="n">
-        <v>39.959</v>
+        <v>49.55</v>
       </c>
       <c r="F22" s="1" t="n">
-        <v>4.074</v>
+        <v>3.482</v>
       </c>
       <c r="G22" t="n">
-        <v>4.239</v>
+        <v>3.741</v>
       </c>
       <c r="H22" t="n">
-        <v>4.4</v>
+        <v>4.165</v>
       </c>
     </row>
     <row r="23">
@@ -848,25 +848,25 @@
         <v>30</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>446.43</v>
+        <v>0.038</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>543.7809999999999</v>
+        <v>98.67700000000001</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>617.864</v>
+        <v>546.926</v>
       </c>
       <c r="E23" s="1" t="n">
-        <v>50.938</v>
+        <v>197.694</v>
       </c>
       <c r="F23" s="1" t="n">
-        <v>30.074</v>
+        <v>24.411</v>
       </c>
       <c r="G23" t="n">
-        <v>31.088</v>
+        <v>25.625</v>
       </c>
       <c r="H23" t="n">
-        <v>32.174</v>
+        <v>26.942</v>
       </c>
     </row>
     <row r="24">
@@ -874,25 +874,25 @@
         <v>50</v>
       </c>
       <c r="B24" s="1" t="n">
-        <v>989.727</v>
+        <v>0.511</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>1056.827</v>
+        <v>719.646</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>1130.995</v>
+        <v>1123.076</v>
       </c>
       <c r="E24" s="1" t="n">
-        <v>43.659</v>
+        <v>476.124</v>
       </c>
       <c r="F24" s="1" t="n">
-        <v>80.224</v>
+        <v>68.542</v>
       </c>
       <c r="G24" t="n">
-        <v>82.98699999999999</v>
+        <v>75.956</v>
       </c>
       <c r="H24" t="n">
-        <v>85.14100000000001</v>
+        <v>87.59099999999999</v>
       </c>
     </row>
     <row r="25">
@@ -957,25 +957,25 @@
         <v>10</v>
       </c>
       <c r="B28" s="1" t="n">
-        <v>93.831</v>
+        <v>10.945</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>206250.984</v>
+        <v>21074.108</v>
       </c>
       <c r="D28" s="1" t="n">
-        <v>364318.054</v>
+        <v>210531.148</v>
       </c>
       <c r="E28" s="1" t="n">
-        <v>119098.041</v>
+        <v>63152.347</v>
       </c>
       <c r="F28" s="1" t="n">
-        <v>3.78</v>
+        <v>3.291</v>
       </c>
       <c r="G28" t="n">
-        <v>3.872</v>
+        <v>3.429</v>
       </c>
       <c r="H28" t="n">
-        <v>3.971</v>
+        <v>3.678</v>
       </c>
     </row>
     <row r="29">
@@ -983,25 +983,25 @@
         <v>30</v>
       </c>
       <c r="B29" s="1" t="n">
-        <v>1262383.423</v>
+        <v>130.234</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>1518041.319</v>
+        <v>485757.737</v>
       </c>
       <c r="D29" s="1" t="n">
-        <v>1809166.501</v>
+        <v>1663701.346</v>
       </c>
       <c r="E29" s="1" t="n">
-        <v>179280.57</v>
+        <v>741979.458</v>
       </c>
       <c r="F29" s="1" t="n">
-        <v>28.632</v>
+        <v>24.223</v>
       </c>
       <c r="G29" t="n">
-        <v>29.165</v>
+        <v>24.993</v>
       </c>
       <c r="H29" t="n">
-        <v>30.322</v>
+        <v>25.896</v>
       </c>
     </row>
     <row r="30">
@@ -1009,25 +1009,25 @@
         <v>50</v>
       </c>
       <c r="B30" s="1" t="n">
-        <v>2741063.758</v>
+        <v>36074.024</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>3172679.587</v>
+        <v>2738934.314</v>
       </c>
       <c r="D30" s="1" t="n">
-        <v>3389324.577</v>
+        <v>3410228.831</v>
       </c>
       <c r="E30" s="1" t="n">
-        <v>196937.608</v>
+        <v>930837.737</v>
       </c>
       <c r="F30" s="1" t="n">
-        <v>76.726</v>
+        <v>63.866</v>
       </c>
       <c r="G30" t="n">
-        <v>78.09399999999999</v>
+        <v>67.88500000000001</v>
       </c>
       <c r="H30" t="n">
-        <v>80.235</v>
+        <v>71.50700000000001</v>
       </c>
     </row>
     <row r="31">
@@ -1092,25 +1092,25 @@
         <v>10</v>
       </c>
       <c r="B34" s="1" t="n">
-        <v>12.3</v>
+        <v>-3.065</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>3863847.826</v>
+        <v>2752550.401</v>
       </c>
       <c r="D34" s="1" t="n">
-        <v>18455086.861</v>
+        <v>26766793.87</v>
       </c>
       <c r="E34" s="1" t="n">
-        <v>5494331.53</v>
+        <v>8007943.506</v>
       </c>
       <c r="F34" s="1" t="n">
-        <v>7.965</v>
+        <v>5.971</v>
       </c>
       <c r="G34" t="n">
-        <v>8.321999999999999</v>
+        <v>6.557</v>
       </c>
       <c r="H34" t="n">
-        <v>8.760999999999999</v>
+        <v>7.31</v>
       </c>
     </row>
     <row r="35">
@@ -1118,25 +1118,25 @@
         <v>30</v>
       </c>
       <c r="B35" s="1" t="n">
-        <v>208679432.699</v>
+        <v>-1.018</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>441762958.29</v>
+        <v>316285208.576</v>
       </c>
       <c r="D35" s="1" t="n">
-        <v>615676602.46</v>
+        <v>585142659.725</v>
       </c>
       <c r="E35" s="1" t="n">
-        <v>105949769.312</v>
+        <v>231936289.151</v>
       </c>
       <c r="F35" s="1" t="n">
-        <v>65.405</v>
+        <v>48.039</v>
       </c>
       <c r="G35" t="n">
-        <v>67.39100000000001</v>
+        <v>56.525</v>
       </c>
       <c r="H35" t="n">
-        <v>70.60599999999999</v>
+        <v>63.648</v>
       </c>
     </row>
     <row r="36">
@@ -1144,25 +1144,25 @@
         <v>50</v>
       </c>
       <c r="B36" s="1" t="n">
-        <v>817405757.696</v>
+        <v>1.539</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>1031807824.065</v>
+        <v>765617344.123</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>1221361116.583</v>
+        <v>1395377722.226</v>
       </c>
       <c r="E36" s="1" t="n">
-        <v>121164612.685</v>
+        <v>527510245.444</v>
       </c>
       <c r="F36" s="1" t="n">
-        <v>179.077</v>
+        <v>129.332</v>
       </c>
       <c r="G36" t="n">
-        <v>183.083</v>
+        <v>145.234</v>
       </c>
       <c r="H36" t="n">
-        <v>189.299</v>
+        <v>165.223</v>
       </c>
     </row>
     <row r="37">

</xml_diff>